<commit_message>
new update - generate bill and upload salary estimate
</commit_message>
<xml_diff>
--- a/customTemplate/vendorBill/customTemplateBill.xlsx
+++ b/customTemplate/vendorBill/customTemplateBill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab0ca60d3e11cd5c/Desktop/hrManagementSystem/customTemplate/vendorBill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_F25DC773A252ABDACC1048B5D95D7FD85BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5D07404-A184-4AAA-9EC0-FFF3FECBBE7C}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_F25DC773A252ABDACC1048B5D95D7FD85BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA256A0E-0D85-4A54-A304-C3EB50131E13}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
   <si>
     <t xml:space="preserve">SUMMARY OF WAGES BILL </t>
   </si>
@@ -261,9 +261,6 @@
     <t xml:space="preserve">Monthly Horticulture Charges </t>
   </si>
   <si>
-    <t xml:space="preserve">Monthely Air Filler Charges </t>
-  </si>
-  <si>
     <t>(D) Other Expenses Reimbursements</t>
   </si>
   <si>
@@ -325,12 +322,6 @@
   </si>
   <si>
     <t>Mediclaim</t>
-  </si>
-  <si>
-    <t>Water Tanker Charges</t>
-  </si>
-  <si>
-    <t>Telephone Bill for EDC</t>
   </si>
 </sst>
 </file>
@@ -513,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1004,49 +995,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1178,7 +1126,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1381,9 +1329,6 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1432,7 +1377,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1444,9 +1389,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1600,16 +1542,10 @@
     <xf numFmtId="1" fontId="13" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1621,34 +1557,34 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1660,7 +1596,7 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="4" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="4" borderId="48" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1669,7 +1605,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1687,7 +1623,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1986,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y75"/>
+  <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1998,17 +1934,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="92"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="90"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2030,16 +1966,16 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="96" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="98"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="96"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2061,32 +1997,32 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="99" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="101"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="99"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="108"/>
+      <c r="Y3" s="108"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -2095,52 +2031,52 @@
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="101"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="99"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="111" t="s">
+      <c r="M4" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="113" t="s">
+      <c r="N4" s="110"/>
+      <c r="O4" s="110"/>
+      <c r="P4" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="111" t="s">
+      <c r="T4" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="114" t="s">
+      <c r="U4" s="110"/>
+      <c r="V4" s="110"/>
+      <c r="W4" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="114"/>
-      <c r="Y4" s="114"/>
+      <c r="X4" s="112"/>
+      <c r="Y4" s="112"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="104"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="106" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="106"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="101"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="99"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -2186,13 +2122,13 @@
       <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="109" t="s">
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="109"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
@@ -2238,13 +2174,13 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="117"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="115"/>
       <c r="F7" s="17" t="s">
         <v>17</v>
       </c>
@@ -2310,13 +2246,13 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -2372,13 +2308,13 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -2422,23 +2358,23 @@
       <c r="Y9" s="7"/>
     </row>
     <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="102" t="s">
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="103"/>
+      <c r="I10" s="101"/>
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="1"/>
@@ -2469,8 +2405,8 @@
       <c r="Y10" s="7"/>
     </row>
     <row r="11" spans="1:25" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="122"/>
-      <c r="B11" s="124"/>
+      <c r="A11" s="120"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="30" t="s">
         <v>25</v>
       </c>
@@ -2499,11 +2435,11 @@
         <v>31</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="116" t="s">
+      <c r="M11" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
+      <c r="N11" s="114"/>
+      <c r="O11" s="114"/>
       <c r="P11" s="36" t="s">
         <v>25</v>
       </c>
@@ -2559,11 +2495,11 @@
         <v>0</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="126" t="s">
+      <c r="M12" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="126"/>
-      <c r="O12" s="126"/>
+      <c r="N12" s="124"/>
+      <c r="O12" s="124"/>
       <c r="P12" s="45">
         <f>+C12</f>
         <v>0</v>
@@ -2579,10 +2515,10 @@
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
-      <c r="V12" s="127"/>
-      <c r="W12" s="127"/>
-      <c r="X12" s="127"/>
-      <c r="Y12" s="127"/>
+      <c r="V12" s="125"/>
+      <c r="W12" s="125"/>
+      <c r="X12" s="125"/>
+      <c r="Y12" s="125"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="46">
@@ -2622,11 +2558,11 @@
         <v>0</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="126" t="s">
+      <c r="M13" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="126"/>
-      <c r="O13" s="126"/>
+      <c r="N13" s="124"/>
+      <c r="O13" s="124"/>
       <c r="P13" s="45">
         <f t="shared" ref="P13:P41" si="3">+C13</f>
         <v>0</v>
@@ -2664,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="42">
-        <f t="shared" si="0"/>
+        <f>D14+E14-C14</f>
         <v>0</v>
       </c>
       <c r="G14" s="43" t="e">
@@ -2685,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="126" t="s">
+      <c r="M14" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="126"/>
-      <c r="O14" s="126"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
       <c r="P14" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2727,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F15:F17" si="6">D15+E15-C15</f>
         <v>0</v>
       </c>
       <c r="G15" s="43" t="e">
@@ -2748,11 +2684,11 @@
         <v>0</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="126" t="s">
+      <c r="M15" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="126"/>
-      <c r="O15" s="126"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
       <c r="P15" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2790,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G16" s="43" t="e">
@@ -2811,11 +2747,11 @@
         <v>0</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="126" t="s">
+      <c r="M16" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="126"/>
-      <c r="O16" s="126"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
       <c r="P16" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2853,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G17" s="43" t="e">
@@ -2874,11 +2810,11 @@
         <v>0</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="126" t="s">
+      <c r="M17" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="126"/>
-      <c r="O17" s="126"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="124"/>
       <c r="P17" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2937,11 +2873,11 @@
         <v>0</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="126" t="s">
+      <c r="M18" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="126"/>
-      <c r="O18" s="126"/>
+      <c r="N18" s="124"/>
+      <c r="O18" s="124"/>
       <c r="P18" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3000,11 +2936,11 @@
         <v>0</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="126" t="s">
+      <c r="M19" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="126"/>
-      <c r="O19" s="126"/>
+      <c r="N19" s="124"/>
+      <c r="O19" s="124"/>
       <c r="P19" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3046,14 +2982,14 @@
         <v>0</v>
       </c>
       <c r="G20" s="43">
-        <f t="shared" ref="G20:G29" si="6">F20*J20/26</f>
+        <f t="shared" ref="G20:G29" si="7">F20*J20/26</f>
         <v>0</v>
       </c>
       <c r="H20" s="41">
         <v>0</v>
       </c>
       <c r="I20" s="44">
-        <f t="shared" ref="I20:I29" si="7">H20*K20/26</f>
+        <f t="shared" ref="I20:I29" si="8">H20*K20/26</f>
         <v>0</v>
       </c>
       <c r="J20" s="35">
@@ -3063,11 +2999,11 @@
         <v>0</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="126" t="s">
+      <c r="M20" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="N20" s="126"/>
-      <c r="O20" s="126"/>
+      <c r="N20" s="124"/>
+      <c r="O20" s="124"/>
       <c r="P20" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3109,14 +3045,14 @@
         <v>0</v>
       </c>
       <c r="G21" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H21" s="41">
         <v>0</v>
       </c>
       <c r="I21" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J21" s="35">
@@ -3126,11 +3062,11 @@
         <v>0</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="126" t="s">
+      <c r="M21" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="N21" s="126"/>
-      <c r="O21" s="126"/>
+      <c r="N21" s="124"/>
+      <c r="O21" s="124"/>
       <c r="P21" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3172,14 +3108,14 @@
         <v>0</v>
       </c>
       <c r="G22" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H22" s="41">
         <v>0</v>
       </c>
       <c r="I22" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J22" s="35">
@@ -3189,11 +3125,11 @@
         <v>0</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="126" t="s">
+      <c r="M22" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="126"/>
-      <c r="O22" s="126"/>
+      <c r="N22" s="124"/>
+      <c r="O22" s="124"/>
       <c r="P22" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3235,14 +3171,14 @@
         <v>0</v>
       </c>
       <c r="G23" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H23" s="41">
         <v>0</v>
       </c>
       <c r="I23" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J23" s="35">
@@ -3252,11 +3188,11 @@
         <v>0</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="126" t="s">
+      <c r="M23" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="N23" s="126"/>
-      <c r="O23" s="126"/>
+      <c r="N23" s="124"/>
+      <c r="O23" s="124"/>
       <c r="P23" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3298,14 +3234,14 @@
         <v>0</v>
       </c>
       <c r="G24" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H24" s="41">
         <v>0</v>
       </c>
       <c r="I24" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J24" s="35">
@@ -3315,11 +3251,11 @@
         <v>0</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="126" t="s">
+      <c r="M24" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
+      <c r="N24" s="124"/>
+      <c r="O24" s="124"/>
       <c r="P24" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3361,14 +3297,14 @@
         <v>0</v>
       </c>
       <c r="G25" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H25" s="41">
         <v>0</v>
       </c>
       <c r="I25" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J25" s="35">
@@ -3378,11 +3314,11 @@
         <v>0</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="126" t="s">
+      <c r="M25" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="N25" s="126"/>
-      <c r="O25" s="126"/>
+      <c r="N25" s="124"/>
+      <c r="O25" s="124"/>
       <c r="P25" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3424,14 +3360,14 @@
         <v>0</v>
       </c>
       <c r="G26" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H26" s="41">
         <v>0</v>
       </c>
       <c r="I26" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J26" s="35">
@@ -3441,11 +3377,11 @@
         <v>0</v>
       </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="126" t="s">
+      <c r="M26" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="N26" s="126"/>
-      <c r="O26" s="126"/>
+      <c r="N26" s="124"/>
+      <c r="O26" s="124"/>
       <c r="P26" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3487,14 +3423,14 @@
         <v>0</v>
       </c>
       <c r="G27" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H27" s="41">
         <v>0</v>
       </c>
       <c r="I27" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J27" s="35">
@@ -3504,11 +3440,11 @@
         <v>0</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="126" t="s">
+      <c r="M27" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="N27" s="126"/>
-      <c r="O27" s="126"/>
+      <c r="N27" s="124"/>
+      <c r="O27" s="124"/>
       <c r="P27" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3550,14 +3486,14 @@
         <v>0</v>
       </c>
       <c r="G28" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H28" s="41">
         <v>0</v>
       </c>
       <c r="I28" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J28" s="35">
@@ -3567,11 +3503,11 @@
         <v>0</v>
       </c>
       <c r="L28" s="1"/>
-      <c r="M28" s="126" t="s">
+      <c r="M28" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="126"/>
-      <c r="O28" s="126"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
       <c r="P28" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3613,14 +3549,14 @@
         <v>0</v>
       </c>
       <c r="G29" s="43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H29" s="41">
         <v>0</v>
       </c>
       <c r="I29" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J29" s="35">
@@ -3630,11 +3566,11 @@
         <v>0</v>
       </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="126" t="s">
+      <c r="M29" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="126"/>
-      <c r="O29" s="126"/>
+      <c r="N29" s="124"/>
+      <c r="O29" s="124"/>
       <c r="P29" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3693,11 +3629,11 @@
         <v>0</v>
       </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="126" t="s">
+      <c r="M30" s="124" t="s">
         <v>51</v>
       </c>
-      <c r="N30" s="126"/>
-      <c r="O30" s="126"/>
+      <c r="N30" s="124"/>
+      <c r="O30" s="124"/>
       <c r="P30" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3756,11 +3692,11 @@
         <v>0</v>
       </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="126" t="s">
+      <c r="M31" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="N31" s="126"/>
-      <c r="O31" s="126"/>
+      <c r="N31" s="124"/>
+      <c r="O31" s="124"/>
       <c r="P31" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3819,11 +3755,11 @@
         <v>0</v>
       </c>
       <c r="L32" s="1"/>
-      <c r="M32" s="126" t="s">
+      <c r="M32" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="N32" s="126"/>
-      <c r="O32" s="126"/>
+      <c r="N32" s="124"/>
+      <c r="O32" s="124"/>
       <c r="P32" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3882,11 +3818,11 @@
         <v>0</v>
       </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="126" t="s">
+      <c r="M33" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="N33" s="126"/>
-      <c r="O33" s="126"/>
+      <c r="N33" s="124"/>
+      <c r="O33" s="124"/>
       <c r="P33" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3945,11 +3881,11 @@
         <v>0</v>
       </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="126" t="s">
+      <c r="M34" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="N34" s="126"/>
-      <c r="O34" s="126"/>
+      <c r="N34" s="124"/>
+      <c r="O34" s="124"/>
       <c r="P34" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4008,11 +3944,11 @@
         <v>0</v>
       </c>
       <c r="L35" s="1"/>
-      <c r="M35" s="126" t="s">
+      <c r="M35" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="N35" s="126"/>
-      <c r="O35" s="126"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="124"/>
       <c r="P35" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4071,11 +4007,11 @@
         <v>0</v>
       </c>
       <c r="L36" s="1"/>
-      <c r="M36" s="126" t="s">
+      <c r="M36" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="N36" s="126"/>
-      <c r="O36" s="126"/>
+      <c r="N36" s="124"/>
+      <c r="O36" s="124"/>
       <c r="P36" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4124,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="44">
-        <f t="shared" ref="I37:I41" si="8">H37*K37/26</f>
+        <f t="shared" ref="I37:I41" si="9">H37*K37/26</f>
         <v>0</v>
       </c>
       <c r="J37" s="35">
@@ -4134,11 +4070,11 @@
         <v>0</v>
       </c>
       <c r="L37" s="1"/>
-      <c r="M37" s="126" t="s">
+      <c r="M37" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="N37" s="126"/>
-      <c r="O37" s="126"/>
+      <c r="N37" s="124"/>
+      <c r="O37" s="124"/>
       <c r="P37" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4180,14 +4116,14 @@
         <v>0</v>
       </c>
       <c r="G38" s="43">
-        <f t="shared" ref="G38:G41" si="9">F38*J38/26</f>
+        <f t="shared" ref="G38:G41" si="10">F38*J38/26</f>
         <v>0</v>
       </c>
       <c r="H38" s="41">
         <v>0</v>
       </c>
       <c r="I38" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J38" s="35">
@@ -4197,11 +4133,11 @@
         <v>0</v>
       </c>
       <c r="L38" s="1"/>
-      <c r="M38" s="126" t="s">
+      <c r="M38" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="N38" s="126"/>
-      <c r="O38" s="126"/>
+      <c r="N38" s="124"/>
+      <c r="O38" s="124"/>
       <c r="P38" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4243,16 +4179,16 @@
         <v>0</v>
       </c>
       <c r="G39" s="43">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="41">
+        <v>0</v>
+      </c>
+      <c r="I39" s="44">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H39" s="41">
-        <v>0</v>
-      </c>
-      <c r="I39" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="J39" s="35">
         <v>0</v>
       </c>
@@ -4260,11 +4196,11 @@
         <v>0</v>
       </c>
       <c r="L39" s="1"/>
-      <c r="M39" s="126" t="s">
+      <c r="M39" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="N39" s="126"/>
-      <c r="O39" s="126"/>
+      <c r="N39" s="124"/>
+      <c r="O39" s="124"/>
       <c r="P39" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4306,16 +4242,16 @@
         <v>0</v>
       </c>
       <c r="G40" s="43">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="41">
+        <v>0</v>
+      </c>
+      <c r="I40" s="44">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H40" s="41">
-        <v>0</v>
-      </c>
-      <c r="I40" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="J40" s="35">
         <v>0</v>
       </c>
@@ -4323,11 +4259,11 @@
         <v>0</v>
       </c>
       <c r="L40" s="1"/>
-      <c r="M40" s="126" t="s">
+      <c r="M40" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="N40" s="126"/>
-      <c r="O40" s="126"/>
+      <c r="N40" s="124"/>
+      <c r="O40" s="124"/>
       <c r="P40" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4369,16 +4305,16 @@
         <v>0</v>
       </c>
       <c r="G41" s="43">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="41">
+        <v>0</v>
+      </c>
+      <c r="I41" s="44">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H41" s="41">
-        <v>0</v>
-      </c>
-      <c r="I41" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="J41" s="35">
         <v>0</v>
       </c>
@@ -4386,11 +4322,11 @@
         <v>0</v>
       </c>
       <c r="L41" s="1"/>
-      <c r="M41" s="126" t="s">
+      <c r="M41" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="N41" s="126"/>
-      <c r="O41" s="126"/>
+      <c r="N41" s="124"/>
+      <c r="O41" s="124"/>
       <c r="P41" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -4428,9 +4364,9 @@
       <c r="J42" s="54"/>
       <c r="K42" s="54"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="131"/>
-      <c r="N42" s="131"/>
-      <c r="O42" s="131"/>
+      <c r="M42" s="129"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="129"/>
       <c r="P42" s="55"/>
       <c r="Q42" s="55"/>
       <c r="R42" s="1"/>
@@ -4567,13 +4503,13 @@
       <c r="Y46" s="1"/>
     </row>
     <row r="47" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="132" t="s">
+      <c r="A47" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="133"/>
-      <c r="C47" s="133"/>
-      <c r="D47" s="133"/>
-      <c r="E47" s="134"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="131"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="132"/>
       <c r="F47" s="62">
         <f>+F12+F14+F16</f>
         <v>0</v>
@@ -4608,13 +4544,13 @@
       <c r="Y47" s="1"/>
     </row>
     <row r="48" spans="1:25" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="135" t="s">
+      <c r="A48" s="133" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="136"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="137"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="135"/>
       <c r="F48" s="64" t="e">
         <f>+G47+I47</f>
         <v>#DIV/0!</v>
@@ -4640,17 +4576,17 @@
       <c r="Y48" s="1"/>
     </row>
     <row r="49" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="128" t="s">
+      <c r="A49" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="129"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="129"/>
-      <c r="E49" s="129"/>
-      <c r="F49" s="129"/>
-      <c r="G49" s="129"/>
-      <c r="H49" s="129"/>
-      <c r="I49" s="130"/>
+      <c r="B49" s="127"/>
+      <c r="C49" s="127"/>
+      <c r="D49" s="127"/>
+      <c r="E49" s="127"/>
+      <c r="F49" s="127"/>
+      <c r="G49" s="127"/>
+      <c r="H49" s="127"/>
+      <c r="I49" s="128"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -4669,22 +4605,22 @@
       <c r="Y49" s="1"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="138" t="s">
+      <c r="B50" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="138"/>
-      <c r="D50" s="138"/>
-      <c r="E50" s="138"/>
-      <c r="F50" s="138"/>
-      <c r="G50" s="138"/>
+      <c r="C50" s="136"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="136"/>
       <c r="H50" s="66">
         <v>0</v>
       </c>
-      <c r="I50" s="139">
-        <f>SUM(H50:H53)</f>
+      <c r="I50" s="137">
+        <f>SUM(H50:H52)</f>
         <v>0</v>
       </c>
       <c r="J50" s="1"/>
@@ -4705,19 +4641,19 @@
       <c r="Y50" s="1"/>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A51" s="86"/>
-      <c r="B51" s="84" t="s">
+      <c r="A51" s="85"/>
+      <c r="B51" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="84"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="84"/>
-      <c r="G51" s="84"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
       <c r="H51" s="67">
         <v>0</v>
       </c>
-      <c r="I51" s="140"/>
+      <c r="I51" s="138"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -4735,20 +4671,20 @@
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A52" s="86"/>
-      <c r="B52" s="84" t="s">
+    <row r="52" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="85"/>
+      <c r="B52" s="83" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
+      <c r="C52" s="83"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
       <c r="H52" s="67">
         <v>0</v>
       </c>
-      <c r="I52" s="140"/>
+      <c r="I52" s="138"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -4767,25 +4703,23 @@
       <c r="Y52" s="1"/>
     </row>
     <row r="53" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="86"/>
-      <c r="B53" s="142" t="s">
+      <c r="A53" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="142"/>
-      <c r="D53" s="142"/>
-      <c r="E53" s="142"/>
-      <c r="F53" s="142"/>
-      <c r="G53" s="142"/>
-      <c r="H53" s="68">
-        <v>0</v>
-      </c>
-      <c r="I53" s="141"/>
+      <c r="B53" s="141"/>
+      <c r="C53" s="141"/>
+      <c r="D53" s="141"/>
+      <c r="E53" s="141"/>
+      <c r="F53" s="141"/>
+      <c r="G53" s="141"/>
+      <c r="H53" s="141"/>
+      <c r="I53" s="142"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
+      <c r="M53" s="68"/>
+      <c r="N53" s="68"/>
+      <c r="O53" s="69"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
@@ -4797,24 +4731,31 @@
       <c r="X53" s="1"/>
       <c r="Y53" s="1"/>
     </row>
-    <row r="54" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="128" t="s">
+    <row r="54" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="145"/>
-      <c r="C54" s="145"/>
-      <c r="D54" s="145"/>
-      <c r="E54" s="145"/>
-      <c r="F54" s="145"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="145"/>
-      <c r="I54" s="146"/>
+      <c r="B54" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="83"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="83"/>
+      <c r="H54" s="81">
+        <v>0</v>
+      </c>
+      <c r="I54" s="86">
+        <f>SUM(H54:H61)</f>
+        <v>0</v>
+      </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="69"/>
-      <c r="N54" s="69"/>
-      <c r="O54" s="70"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="69"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
@@ -4826,31 +4767,26 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="1"/>
     </row>
-    <row r="55" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="84" t="s">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A55" s="85"/>
+      <c r="B55" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84"/>
-      <c r="G55" s="84"/>
-      <c r="H55" s="82">
-        <v>0</v>
-      </c>
-      <c r="I55" s="87">
-        <f>SUM(H55:H64)</f>
-        <v>0</v>
-      </c>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="81">
+        <v>0</v>
+      </c>
+      <c r="I55" s="87"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="69"/>
-      <c r="N55" s="69"/>
-      <c r="O55" s="70"/>
+      <c r="M55" s="68"/>
+      <c r="N55" s="68"/>
+      <c r="O55" s="69"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -4863,25 +4799,25 @@
       <c r="Y55" s="1"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A56" s="86"/>
-      <c r="B56" s="84" t="s">
+      <c r="A56" s="85"/>
+      <c r="B56" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="84"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="84"/>
-      <c r="F56" s="84"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="82">
-        <v>0</v>
-      </c>
-      <c r="I56" s="88"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="83"/>
+      <c r="E56" s="83"/>
+      <c r="F56" s="83"/>
+      <c r="G56" s="83"/>
+      <c r="H56" s="81">
+        <v>0</v>
+      </c>
+      <c r="I56" s="87"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-      <c r="M56" s="69"/>
-      <c r="N56" s="69"/>
-      <c r="O56" s="70"/>
+      <c r="M56" s="68"/>
+      <c r="N56" s="68"/>
+      <c r="O56" s="69"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -4894,25 +4830,25 @@
       <c r="Y56" s="1"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A57" s="86"/>
-      <c r="B57" s="84" t="s">
+      <c r="A57" s="85"/>
+      <c r="B57" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="84"/>
-      <c r="G57" s="84"/>
-      <c r="H57" s="82">
-        <v>0</v>
-      </c>
-      <c r="I57" s="88"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="83"/>
+      <c r="E57" s="83"/>
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="81">
+        <v>0</v>
+      </c>
+      <c r="I57" s="87"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="69"/>
-      <c r="N57" s="69"/>
-      <c r="O57" s="70"/>
+      <c r="M57" s="68"/>
+      <c r="N57" s="68"/>
+      <c r="O57" s="69"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -4925,25 +4861,25 @@
       <c r="Y57" s="1"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A58" s="86"/>
-      <c r="B58" s="84" t="s">
+      <c r="A58" s="85"/>
+      <c r="B58" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="84"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="84"/>
-      <c r="F58" s="84"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="82">
-        <v>0</v>
-      </c>
-      <c r="I58" s="88"/>
+      <c r="C58" s="83"/>
+      <c r="D58" s="83"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="83"/>
+      <c r="H58" s="81">
+        <v>0</v>
+      </c>
+      <c r="I58" s="87"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="69"/>
-      <c r="N58" s="69"/>
-      <c r="O58" s="70"/>
+      <c r="M58" s="68"/>
+      <c r="N58" s="68"/>
+      <c r="O58" s="69"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -4956,25 +4892,25 @@
       <c r="Y58" s="1"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A59" s="86"/>
-      <c r="B59" s="84" t="s">
+      <c r="A59" s="85"/>
+      <c r="B59" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="84"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="84"/>
-      <c r="F59" s="84"/>
-      <c r="G59" s="84"/>
-      <c r="H59" s="82">
-        <v>0</v>
-      </c>
-      <c r="I59" s="88"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="81">
+        <v>0</v>
+      </c>
+      <c r="I59" s="87"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="69"/>
-      <c r="N59" s="69"/>
-      <c r="O59" s="70"/>
+      <c r="M59" s="68"/>
+      <c r="N59" s="68"/>
+      <c r="O59" s="69"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -4987,25 +4923,25 @@
       <c r="Y59" s="1"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A60" s="86"/>
-      <c r="B60" s="84" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="84"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="84"/>
-      <c r="F60" s="84"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="82">
-        <v>0</v>
-      </c>
-      <c r="I60" s="88"/>
+      <c r="A60" s="85"/>
+      <c r="B60" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="83"/>
+      <c r="D60" s="83"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="83"/>
+      <c r="H60" s="81">
+        <v>0</v>
+      </c>
+      <c r="I60" s="87"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="69"/>
-      <c r="N60" s="69"/>
-      <c r="O60" s="70"/>
+      <c r="M60" s="68"/>
+      <c r="N60" s="68"/>
+      <c r="O60" s="69"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5017,26 +4953,26 @@
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A61" s="86"/>
-      <c r="B61" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="84"/>
-      <c r="G61" s="84"/>
+    <row r="61" spans="1:25" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="85"/>
+      <c r="B61" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="83"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="83"/>
       <c r="H61" s="82">
         <v>0</v>
       </c>
-      <c r="I61" s="88"/>
+      <c r="I61" s="87"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="69"/>
-      <c r="N61" s="69"/>
-      <c r="O61" s="70"/>
+      <c r="M61" s="68"/>
+      <c r="N61" s="68"/>
+      <c r="O61" s="69"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5048,26 +4984,24 @@
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
     </row>
-    <row r="62" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="86"/>
-      <c r="B62" s="84" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="84"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="84"/>
-      <c r="F62" s="84"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="83">
-        <v>0</v>
-      </c>
-      <c r="I62" s="88"/>
+    <row r="62" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="143" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="144"/>
+      <c r="C62" s="144"/>
+      <c r="D62" s="144"/>
+      <c r="E62" s="144"/>
+      <c r="F62" s="144"/>
+      <c r="G62" s="144"/>
+      <c r="H62" s="145"/>
+      <c r="I62" s="146"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="69"/>
-      <c r="N62" s="69"/>
-      <c r="O62" s="70"/>
+      <c r="N62" s="68"/>
+      <c r="O62" s="69"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5080,25 +5014,30 @@
       <c r="Y62" s="1"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A63" s="86"/>
-      <c r="B63" s="84" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="84"/>
-      <c r="F63" s="84"/>
-      <c r="G63" s="84"/>
-      <c r="H63" s="83">
-        <v>0</v>
-      </c>
-      <c r="I63" s="88"/>
+      <c r="A63" s="147" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="149" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="149"/>
+      <c r="D63" s="149"/>
+      <c r="E63" s="149"/>
+      <c r="F63" s="149"/>
+      <c r="G63" s="150"/>
+      <c r="H63" s="70">
+        <v>0</v>
+      </c>
+      <c r="I63" s="151">
+        <f>SUM(H63:H64)</f>
+        <v>0</v>
+      </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="69"/>
       <c r="N63" s="69"/>
-      <c r="O63" s="70"/>
+      <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -5111,25 +5050,25 @@
       <c r="Y63" s="1"/>
     </row>
     <row r="64" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="86"/>
-      <c r="B64" s="84" t="s">
-        <v>98</v>
-      </c>
-      <c r="C64" s="84"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="84"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="83">
-        <v>0</v>
-      </c>
-      <c r="I64" s="89"/>
+      <c r="A64" s="148"/>
+      <c r="B64" s="152" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="152"/>
+      <c r="D64" s="152"/>
+      <c r="E64" s="152"/>
+      <c r="F64" s="152"/>
+      <c r="G64" s="153"/>
+      <c r="H64" s="71">
+        <v>0</v>
+      </c>
+      <c r="I64" s="151"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="69"/>
-      <c r="N64" s="69"/>
-      <c r="O64" s="70"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -5142,23 +5081,26 @@
       <c r="Y64" s="1"/>
     </row>
     <row r="65" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="147" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="148"/>
-      <c r="C65" s="148"/>
-      <c r="D65" s="148"/>
-      <c r="E65" s="148"/>
-      <c r="F65" s="148"/>
-      <c r="G65" s="148"/>
-      <c r="H65" s="149"/>
-      <c r="I65" s="150"/>
+      <c r="A65" s="139" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="140"/>
+      <c r="C65" s="140"/>
+      <c r="D65" s="140"/>
+      <c r="E65" s="140"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="140"/>
+      <c r="H65" s="140"/>
+      <c r="I65" s="72" t="e">
+        <f>+F48+I50+I63</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="70"/>
-      <c r="N65" s="69"/>
-      <c r="O65" s="70"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -5171,29 +5113,30 @@
       <c r="Y65" s="1"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A66" s="151" t="s">
-        <v>80</v>
-      </c>
-      <c r="B66" s="153" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="153"/>
-      <c r="D66" s="153"/>
-      <c r="E66" s="153"/>
-      <c r="F66" s="153"/>
-      <c r="G66" s="154"/>
-      <c r="H66" s="71">
-        <v>0</v>
-      </c>
-      <c r="I66" s="155">
-        <f>SUM(H66:H67)</f>
-        <v>0</v>
+      <c r="A66" s="159" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="161" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="162"/>
+      <c r="D66" s="162"/>
+      <c r="E66" s="162"/>
+      <c r="F66" s="162"/>
+      <c r="G66" s="162"/>
+      <c r="H66" s="73" t="e">
+        <f>ROUND(I65*18%,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="137" t="e">
+        <f>H66+H67</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-      <c r="M66" s="70"/>
-      <c r="N66" s="70"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -5207,19 +5150,15 @@
       <c r="Y66" s="1"/>
     </row>
     <row r="67" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="152"/>
-      <c r="B67" s="156" t="s">
-        <v>82</v>
-      </c>
-      <c r="C67" s="156"/>
-      <c r="D67" s="156"/>
-      <c r="E67" s="156"/>
-      <c r="F67" s="156"/>
-      <c r="G67" s="157"/>
-      <c r="H67" s="72">
-        <v>0</v>
-      </c>
-      <c r="I67" s="155"/>
+      <c r="A67" s="160"/>
+      <c r="B67" s="164"/>
+      <c r="C67" s="165"/>
+      <c r="D67" s="165"/>
+      <c r="E67" s="165"/>
+      <c r="F67" s="165"/>
+      <c r="G67" s="165"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="163"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -5238,18 +5177,23 @@
       <c r="Y67" s="1"/>
     </row>
     <row r="68" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="144"/>
-      <c r="C68" s="144"/>
-      <c r="D68" s="144"/>
-      <c r="E68" s="144"/>
-      <c r="F68" s="144"/>
-      <c r="G68" s="144"/>
-      <c r="H68" s="144"/>
-      <c r="I68" s="73" t="e">
-        <f>+F48+I50+I66</f>
+      <c r="A68" s="166" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="167" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="168"/>
+      <c r="D68" s="168"/>
+      <c r="E68" s="168"/>
+      <c r="F68" s="168"/>
+      <c r="G68" s="168"/>
+      <c r="H68" s="75" t="e">
+        <f>+(I65)*1%</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" s="76" t="e">
+        <f>H68</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J68" s="1"/>
@@ -5269,24 +5213,19 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A69" s="163" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="165" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" s="166"/>
-      <c r="D69" s="166"/>
-      <c r="E69" s="166"/>
-      <c r="F69" s="166"/>
-      <c r="G69" s="166"/>
-      <c r="H69" s="74" t="e">
-        <f>ROUND(I68*18%,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I69" s="139" t="e">
-        <f>H69+H70</f>
+    <row r="69" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="160"/>
+      <c r="B69" s="139" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="169"/>
+      <c r="D69" s="169"/>
+      <c r="E69" s="169"/>
+      <c r="F69" s="169"/>
+      <c r="G69" s="169"/>
+      <c r="H69" s="169"/>
+      <c r="I69" s="77" t="e">
+        <f>+I65+I66-I68</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J69" s="1"/>
@@ -5307,15 +5246,15 @@
       <c r="Y69" s="1"/>
     </row>
     <row r="70" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="164"/>
-      <c r="B70" s="168"/>
-      <c r="C70" s="169"/>
-      <c r="D70" s="169"/>
-      <c r="E70" s="169"/>
-      <c r="F70" s="169"/>
-      <c r="G70" s="169"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="167"/>
+      <c r="A70" s="78"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="79"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -5333,26 +5272,21 @@
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
     </row>
-    <row r="71" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="170" t="s">
-        <v>86</v>
-      </c>
-      <c r="B71" s="171" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="172"/>
-      <c r="D71" s="172"/>
-      <c r="E71" s="172"/>
-      <c r="F71" s="172"/>
-      <c r="G71" s="172"/>
-      <c r="H71" s="76" t="e">
-        <f>+(I68)*1%</f>
+    <row r="71" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="154" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="155"/>
+      <c r="C71" s="155"/>
+      <c r="D71" s="155"/>
+      <c r="E71" s="155"/>
+      <c r="F71" s="155"/>
+      <c r="G71" s="156"/>
+      <c r="H71" s="157" t="e">
+        <f>+I69+I54</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I71" s="77" t="e">
-        <f>H71</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I71" s="158"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -5370,21 +5304,16 @@
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
     </row>
-    <row r="72" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="164"/>
-      <c r="B72" s="143" t="s">
-        <v>88</v>
-      </c>
-      <c r="C72" s="173"/>
-      <c r="D72" s="173"/>
-      <c r="E72" s="173"/>
-      <c r="F72" s="173"/>
-      <c r="G72" s="173"/>
-      <c r="H72" s="173"/>
-      <c r="I72" s="78" t="e">
-        <f>+I68+I69-I71</f>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A72" s="80"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -5402,125 +5331,37 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
     </row>
-    <row r="73" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="79"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="80"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-      <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-    </row>
-    <row r="74" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="158" t="s">
-        <v>89</v>
-      </c>
-      <c r="B74" s="159"/>
-      <c r="C74" s="159"/>
-      <c r="D74" s="159"/>
-      <c r="E74" s="159"/>
-      <c r="F74" s="159"/>
-      <c r="G74" s="160"/>
-      <c r="H74" s="161" t="e">
-        <f>+I72+I55</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I74" s="162"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-      <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A75" s="81"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
-      <c r="X75" s="1"/>
-      <c r="Y75" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="A68:H68"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="B62:G62"/>
+  <mergeCells count="96">
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="A65:H65"/>
+    <mergeCell ref="A53:I53"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B54:G54"/>
     <mergeCell ref="B55:G55"/>
     <mergeCell ref="B56:G56"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="B58:G58"/>
     <mergeCell ref="B59:G59"/>
     <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:A64"/>
     <mergeCell ref="B63:G63"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="I63:I64"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="A50:A52"/>
     <mergeCell ref="B50:G50"/>
-    <mergeCell ref="I50:I53"/>
+    <mergeCell ref="I50:I52"/>
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
     <mergeCell ref="A49:I49"/>
     <mergeCell ref="M34:O34"/>
     <mergeCell ref="M35:O35"/>
@@ -5573,9 +5414,8 @@
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="I55:I64"/>
+    <mergeCell ref="A54:A61"/>
+    <mergeCell ref="I54:I61"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -5591,8 +5431,8 @@
     <mergeCell ref="E6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B69" r:id="rId1" display="IGST@18.0%" xr:uid="{F45D5D3F-6C0A-49D2-96C5-34A06D2D3CA4}"/>
-    <hyperlink ref="B71" r:id="rId2" xr:uid="{6A407B9F-84D0-432B-9112-B04D8F163F26}"/>
+    <hyperlink ref="B66" r:id="rId1" display="IGST@18.0%" xr:uid="{F45D5D3F-6C0A-49D2-96C5-34A06D2D3CA4}"/>
+    <hyperlink ref="B68" r:id="rId2" xr:uid="{6A407B9F-84D0-432B-9112-B04D8F163F26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>